<commit_message>
homescreen mit Verarbeitung von Serverinput
Test mit Serverdaten ausstehend (aktuell lokale testdaten im Code!)
</commit_message>
<xml_diff>
--- a/Documents/Phasen/Concept/Nutzung des localStorage.xlsx
+++ b/Documents/Phasen/Concept/Nutzung des localStorage.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="22995" windowHeight="10035"/>
+    <workbookView xWindow="480" yWindow="105" windowWidth="22995" windowHeight="9975"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Local storage</t>
   </si>
@@ -27,9 +27,6 @@
     <t>questions</t>
   </si>
   <si>
-    <t>beinhaltet die durch den Nutzer (nicht Gegner) ausgewählte Kategorie</t>
-  </si>
-  <si>
     <t>Key</t>
   </si>
   <si>
@@ -43,6 +40,21 @@
   </si>
   <si>
     <t>Die wievielte Frage der aktuellen Runde ist es [0;2]</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>enthält die durch den Nutzer (nicht Gegner) ausgewählte Kategorie</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>enthält den nutzernamen des angemeldeten benutzers</t>
+  </si>
+  <si>
+    <t>enthält das passwort des angemeldeten benutzers</t>
   </si>
 </sst>
 </file>
@@ -95,8 +107,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A3:B6" totalsRowShown="0">
-  <autoFilter ref="A3:B6"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A3:B8" totalsRowShown="0">
+  <autoFilter ref="A3:B8"/>
   <tableColumns count="2">
     <tableColumn id="1" name="Key"/>
     <tableColumn id="2" name="Value"/>
@@ -392,10 +404,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -411,10 +423,10 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
         <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -422,7 +434,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -430,15 +442,31 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
         <v>7</v>
       </c>
-      <c r="B6" t="s">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Serverschnittstelle + localStorage-Nutzung aktualisiert.
</commit_message>
<xml_diff>
--- a/Documents/Phasen/Concept/Nutzung des localStorage.xlsx
+++ b/Documents/Phasen/Concept/Nutzung des localStorage.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="22995" windowHeight="9975"/>
+    <workbookView xWindow="480" yWindow="105" windowWidth="19440" windowHeight="9975"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Local storage</t>
   </si>
@@ -55,6 +55,24 @@
   </si>
   <si>
     <t>enthält das passwort des angemeldeten benutzers</t>
+  </si>
+  <si>
+    <t>gameQuestionStart</t>
+  </si>
+  <si>
+    <t>gameQuestionContinue</t>
+  </si>
+  <si>
+    <t>enthält drei Kategorien plus je drei Fragen</t>
+  </si>
+  <si>
+    <t>enthält den aktuellen Datensatz des Spiels, wie er durch sync empfangen wurde</t>
+  </si>
+  <si>
+    <t>gameInfo</t>
+  </si>
+  <si>
+    <t>enthält drei Fragen plus die Antworten des Gegners zu ebendiesen Fragen</t>
   </si>
 </sst>
 </file>
@@ -94,7 +112,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -107,8 +125,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A3:B8" totalsRowShown="0">
-  <autoFilter ref="A3:B8"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A3:B11" totalsRowShown="0">
+  <autoFilter ref="A3:B11"/>
   <tableColumns count="2">
     <tableColumn id="1" name="Key"/>
     <tableColumn id="2" name="Value"/>
@@ -118,9 +136,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Larissa">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -158,7 +176,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Larissa">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -230,7 +248,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Larissa">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -404,13 +422,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="40.42578125" customWidth="1"/>
     <col min="2" max="2" width="65" bestFit="1" customWidth="1"/>
@@ -431,42 +449,66 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>10</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -483,7 +525,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -495,7 +537,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
localstorage: gameOverview & enemyusername
</commit_message>
<xml_diff>
--- a/Documents/Phasen/Concept/Nutzung des localStorage.xlsx
+++ b/Documents/Phasen/Concept/Nutzung des localStorage.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Local storage</t>
   </si>
@@ -79,6 +79,12 @@
   </si>
   <si>
     <t>Enthält ein Array mit ein bis drei Antworten des Spielers, das anschließend zum Server übertragen wird</t>
+  </si>
+  <si>
+    <t>enemyUsername</t>
+  </si>
+  <si>
+    <t>username des gegenspielers</t>
   </si>
 </sst>
 </file>
@@ -118,7 +124,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -131,8 +137,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A3:B12" totalsRowShown="0">
-  <autoFilter ref="A3:B12"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A3:B14" totalsRowShown="0">
+  <autoFilter ref="A3:B14"/>
   <tableColumns count="2">
     <tableColumn id="1" name="Key"/>
     <tableColumn id="2" name="Value"/>
@@ -142,9 +148,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -182,7 +188,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -254,7 +260,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -428,13 +434,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="40.42578125" customWidth="1"/>
     <col min="2" max="2" width="65" bestFit="1" customWidth="1"/>
@@ -525,6 +531,14 @@
         <v>20</v>
       </c>
     </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -539,7 +553,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -551,7 +565,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
LocalStorage: rundenübersicht korrekt laden
</commit_message>
<xml_diff>
--- a/Documents/Phasen/Concept/Nutzung des localStorage.xlsx
+++ b/Documents/Phasen/Concept/Nutzung des localStorage.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Local storage</t>
   </si>
@@ -91,6 +91,13 @@
   </si>
   <si>
     <t>vom Server gelieferte Daten für die Rundenübersicht</t>
+  </si>
+  <si>
+    <t>true: die rundenübersicht wird für dieses Spiel neu aufgerufen (aus hauptmenü heraus)
+false: die rundenübersicht wird lediglich aktualisiert!</t>
+  </si>
+  <si>
+    <t>gameOverviewInitialize</t>
   </si>
 </sst>
 </file>
@@ -126,8 +133,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -143,8 +153,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A3:B14" totalsRowShown="0">
-  <autoFilter ref="A3:B14"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A3:B15" totalsRowShown="0">
+  <autoFilter ref="A3:B15"/>
   <tableColumns count="2">
     <tableColumn id="1" name="Key"/>
     <tableColumn id="2" name="Value"/>
@@ -440,10 +450,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -553,6 +563,14 @@
         <v>24</v>
       </c>
     </row>
+    <row r="15" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>